<commit_message>
Updated project with latest changes
</commit_message>
<xml_diff>
--- a/data/Generate_File/email_data_with_sent_date.xlsx
+++ b/data/Generate_File/email_data_with_sent_date.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11-03-25</t>
+          <t>16-03-25</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>viju</t>
+          <t>Viju</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -495,14 +495,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>11-03-25</t>
+          <t>16-03-25</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>pqr</t>
+          <t>www</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -510,8 +510,16 @@
           <t>Nitin</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nds.nitin@gmail.com </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>16-03-25</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>